<commit_message>
Bill of Materials update.
</commit_message>
<xml_diff>
--- a/AD5791-AD7734/arduino-shield/arduino-shield-bom.xlsx
+++ b/AD5791-AD7734/arduino-shield/arduino-shield-bom.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t xml:space="preserve">PC TEST POINT MINIATURE BLACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3CCH-1018G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assmann WSW Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDC CBL - HHKC10H/AE10G/HHKC10H</t>
   </si>
 </sst>
 </file>
@@ -168,7 +177,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -189,16 +198,135 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -206,8 +334,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,6 +374,23 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -246,14 +406,91 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -262,10 +499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,7 +583,7 @@
       <c r="E3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -386,7 +623,7 @@
       <c r="E5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="0" t="s">
         <v>23</v>
       </c>
     </row>
@@ -489,6 +726,20 @@
       </c>
       <c r="F10" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -496,11 +747,11 @@
     <mergeCell ref="F2:K2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>